<commit_message>
Minor edits to baseline docs (i.e., text/wording)
</commit_message>
<xml_diff>
--- a/MSc_data/Data_new/BenthicCover_BlankSheet_CMA.xlsx
+++ b/MSc_data/Data_new/BenthicCover_BlankSheet_CMA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire\Desktop\MSc\Thesis\kelp_comms_2022\MSc_data\Data_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE5FB36-EEB7-4F3F-B9BD-0F2A7462C2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7244B8AF-E552-4E2D-B44C-8C6590A1EEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AEE024E6-ED02-4460-8513-1C7CB077737A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>SiteName</t>
   </si>
@@ -119,27 +119,15 @@
     <t>Ab_</t>
   </si>
   <si>
-    <t>Counted adundance of an animal species (*Add as needed)</t>
-  </si>
-  <si>
     <t>Ab_Urticina piscivora</t>
   </si>
   <si>
     <t>Image point that is non-algal and a macro biotic organism (e.g., live fish, live inverts, shells...)</t>
   </si>
   <si>
-    <t>Between Scotts and Bradys</t>
-  </si>
-  <si>
     <t>Date that the image was taken at study site (format = month/day/year)</t>
   </si>
   <si>
-    <t>CMA</t>
-  </si>
-  <si>
-    <t>P7052544</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
@@ -237,6 +225,9 @@
   </si>
   <si>
     <t>9 to 32</t>
+  </si>
+  <si>
+    <t>Counted abundance of an animal species (*Add further columns as needed)</t>
   </si>
 </sst>
 </file>
@@ -601,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C35883-A3EF-41F5-AAA8-19EBB5913684}">
   <dimension ref="A1:AR3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AH9" sqref="AH9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,100 +725,100 @@
         <v>7</v>
       </c>
       <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
         <v>34</v>
       </c>
-      <c r="K2" t="s">
+      <c r="P2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>37</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" t="s">
+      <c r="T2" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="U2" t="s">
         <v>40</v>
       </c>
-      <c r="R2" t="s">
+      <c r="V2" t="s">
         <v>41</v>
       </c>
-      <c r="S2" t="s">
+      <c r="W2" t="s">
         <v>42</v>
       </c>
-      <c r="T2" t="s">
+      <c r="X2" t="s">
         <v>43</v>
       </c>
-      <c r="U2" t="s">
+      <c r="Y2" t="s">
         <v>44</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Z2" t="s">
         <v>45</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AA2" t="s">
         <v>46</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AB2" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AC2" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AD2" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AE2" t="s">
         <v>50</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AF2" t="s">
         <v>51</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AG2" t="s">
         <v>52</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AH2" t="s">
         <v>53</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AI2" t="s">
         <v>54</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AJ2" t="s">
         <v>55</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AK2" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AL2" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AM2" t="s">
         <v>58</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AN2" t="s">
         <v>59</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AO2" t="s">
         <v>60</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>64</v>
       </c>
       <c r="AP2" t="s">
         <v>16</v>
@@ -836,25 +827,11 @@
         <v>25</v>
       </c>
       <c r="AR2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="3">
-        <v>44747</v>
-      </c>
-      <c r="C3">
-        <v>2.7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
+      <c r="B3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -867,7 +844,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +865,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -949,7 +926,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -957,15 +934,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -981,7 +958,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -1000,7 +977,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>